<commit_message>
BOT-690 added separate sort field in convo header
</commit_message>
<xml_diff>
--- a/test/convo/convos/partialconvo/excel/convo.xlsx
+++ b/test/convo/convos/partialconvo/excel/convo.xlsx
@@ -44,11 +44,11 @@
   </si>
   <si>
     <t>Login please
-INCLUDE PConvos-B2</t>
+INCLUDE PConvos-A2</t>
   </si>
   <si>
     <t>Logout please!
-INCLUDE PConvos-B5</t>
+INCLUDE PConvos-A5</t>
   </si>
 </sst>
 </file>
@@ -361,7 +361,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -372,7 +372,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -420,7 +420,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
BOT-690 additional logging for wrong partial convo references
</commit_message>
<xml_diff>
--- a/test/convo/convos/partialconvo/excel/convo.xlsx
+++ b/test/convo/convos/partialconvo/excel/convo.xlsx
@@ -55,7 +55,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -63,13 +63,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -84,10 +98,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -361,7 +381,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -372,7 +392,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -382,10 +402,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -420,7 +440,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -430,10 +450,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>